<commit_message>
tambah ba ahda, yandri, wirasandi
</commit_message>
<xml_diff>
--- a/Berita Acara SYMA/27 Oktober 2023 - SYMA - Ahda.xlsx
+++ b/Berita Acara SYMA/27 Oktober 2023 - SYMA - Ahda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Berita Acara Vendor\Berita Acara SYMA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E62AA2-DF50-4552-A8AA-0F5BEF359F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B82A470-5162-47F6-9992-F503569988BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -750,6 +750,56 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
@@ -760,10 +810,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -787,6 +834,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -795,56 +845,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1222,7 +1222,7 @@
   <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:F22"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="11.85" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1310,10 +1310,10 @@
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
       <c r="D9" s="9"/>
-      <c r="G9" s="41">
+      <c r="G9" s="58">
         <v>45226</v>
       </c>
-      <c r="H9" s="41"/>
+      <c r="H9" s="58"/>
       <c r="I9" s="10"/>
       <c r="J9" s="11"/>
     </row>
@@ -1358,50 +1358,50 @@
       <c r="A14" s="15"/>
     </row>
     <row r="15" spans="1:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+      <c r="A15" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="52" t="s">
+      <c r="D15" s="63"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="53" t="s">
+      <c r="G15" s="70" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="54"/>
-      <c r="I15" s="55"/>
-      <c r="J15" s="44" t="s">
+      <c r="H15" s="71"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="51" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="A16" s="43"/>
-      <c r="B16" s="62"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="66"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="66"/>
+      <c r="E16" s="67"/>
+      <c r="F16" s="69"/>
       <c r="G16" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="H16" s="69" t="s">
+      <c r="H16" s="46" t="s">
         <v>13</v>
       </c>
       <c r="I16" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="J16" s="45"/>
+      <c r="J16" s="52"/>
     </row>
     <row r="17" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A17" s="32"/>
-      <c r="B17" s="64" t="s">
+      <c r="B17" s="43" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="33" t="s">
@@ -1409,13 +1409,13 @@
       </c>
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
-      <c r="F17" s="64">
+      <c r="F17" s="43">
         <v>49</v>
       </c>
-      <c r="G17" s="61">
+      <c r="G17" s="41">
         <v>49</v>
       </c>
-      <c r="H17" s="71"/>
+      <c r="H17" s="47"/>
       <c r="I17" s="35">
         <f>SUM(G17:H17)</f>
         <v>49</v>
@@ -1424,7 +1424,7 @@
     </row>
     <row r="18" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A18" s="34"/>
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="44" t="s">
         <v>23</v>
       </c>
       <c r="C18" s="33" t="s">
@@ -1432,13 +1432,13 @@
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
-      <c r="F18" s="68">
+      <c r="F18" s="45">
         <v>2</v>
       </c>
-      <c r="G18" s="61">
+      <c r="G18" s="41">
         <v>2</v>
       </c>
-      <c r="H18" s="72"/>
+      <c r="H18" s="48"/>
       <c r="I18" s="35">
         <f t="shared" ref="I18:I21" si="0">SUM(G18:H18)</f>
         <v>2</v>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="19" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A19" s="34"/>
-      <c r="B19" s="65" t="s">
+      <c r="B19" s="44" t="s">
         <v>27</v>
       </c>
       <c r="C19" s="33" t="s">
@@ -1455,13 +1455,13 @@
       </c>
       <c r="D19" s="34"/>
       <c r="E19" s="34"/>
-      <c r="F19" s="68">
+      <c r="F19" s="45">
         <v>5</v>
       </c>
-      <c r="G19" s="61">
+      <c r="G19" s="41">
         <v>5</v>
       </c>
-      <c r="H19" s="72"/>
+      <c r="H19" s="48"/>
       <c r="I19" s="35">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1470,7 +1470,7 @@
     </row>
     <row r="20" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A20" s="34"/>
-      <c r="B20" s="65" t="s">
+      <c r="B20" s="44" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="33" t="s">
@@ -1478,13 +1478,13 @@
       </c>
       <c r="D20" s="34"/>
       <c r="E20" s="34"/>
-      <c r="F20" s="68">
+      <c r="F20" s="45">
         <v>10</v>
       </c>
-      <c r="G20" s="61">
+      <c r="G20" s="41">
         <v>10</v>
       </c>
-      <c r="H20" s="72"/>
+      <c r="H20" s="48"/>
       <c r="I20" s="35">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="21" spans="1:10" ht="12" x14ac:dyDescent="0.2">
       <c r="A21" s="34"/>
-      <c r="B21" s="65" t="s">
+      <c r="B21" s="44" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="33" t="s">
@@ -1501,13 +1501,13 @@
       </c>
       <c r="D21" s="34"/>
       <c r="E21" s="34"/>
-      <c r="F21" s="68">
+      <c r="F21" s="45">
         <v>1</v>
       </c>
-      <c r="G21" s="61">
+      <c r="G21" s="41">
         <v>1</v>
       </c>
-      <c r="H21" s="72"/>
+      <c r="H21" s="48"/>
       <c r="I21" s="35">
         <f t="shared" si="0"/>
         <v>1</v>
@@ -1515,17 +1515,17 @@
       <c r="J21" s="36"/>
     </row>
     <row r="22" spans="1:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="A22" s="58"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
-      <c r="F22" s="67"/>
+      <c r="A22" s="53"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="55"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="55"/>
+      <c r="F22" s="56"/>
       <c r="G22" s="39">
         <f t="shared" ref="G22:H22" si="1">SUM(G17:G21)</f>
         <v>67</v>
       </c>
-      <c r="H22" s="70">
+      <c r="H22" s="42">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -1545,7 +1545,7 @@
       <c r="F24" s="16"/>
     </row>
     <row r="25" spans="1:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="A25" s="60" t="s">
+      <c r="A25" s="57" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="31"/>
@@ -1553,7 +1553,7 @@
       <c r="D25" s="31"/>
     </row>
     <row r="26" spans="1:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="A26" s="60"/>
+      <c r="A26" s="57"/>
       <c r="B26" s="17"/>
       <c r="C26" s="18"/>
       <c r="D26" s="19"/>
@@ -1631,34 +1631,34 @@
       <c r="B34" s="28"/>
       <c r="C34" s="29"/>
       <c r="D34" s="30"/>
-      <c r="F34" s="41">
+      <c r="F34" s="58">
         <f>G9</f>
         <v>45226</v>
       </c>
-      <c r="G34" s="41"/>
-      <c r="I34" s="41">
+      <c r="G34" s="58"/>
+      <c r="I34" s="58">
         <v>45231</v>
       </c>
-      <c r="J34" s="41"/>
+      <c r="J34" s="58"/>
     </row>
     <row r="35" spans="1:10" ht="12" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I36" s="56"/>
-      <c r="J36" s="56"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
     </row>
     <row r="37" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I37" s="56"/>
-      <c r="J37" s="56"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
     </row>
     <row r="38" spans="1:10" ht="11.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="I38" s="56"/>
-      <c r="J38" s="56"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
     </row>
     <row r="40" spans="1:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="J40" s="57"/>
+      <c r="J40" s="50"/>
     </row>
     <row r="41" spans="1:10" ht="12" x14ac:dyDescent="0.2">
-      <c r="J41" s="57"/>
+      <c r="J41" s="50"/>
     </row>
   </sheetData>
   <protectedRanges>
@@ -1666,6 +1666,12 @@
     <protectedRange sqref="A9:A13" name="Penerimaan_1_1"/>
   </protectedRanges>
   <mergeCells count="15">
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:I15"/>
     <mergeCell ref="I37:J37"/>
     <mergeCell ref="I38:J38"/>
     <mergeCell ref="J40:J41"/>
@@ -1675,12 +1681,6 @@
     <mergeCell ref="F34:G34"/>
     <mergeCell ref="I34:J34"/>
     <mergeCell ref="I36:J36"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:I15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="88" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>